<commit_message>
modifiche per acquisizione dati da file excel -> funzionante script per hybrid house cancellato
</commit_message>
<xml_diff>
--- a/excel_sviluppo.xlsx
+++ b/excel_sviluppo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Commesse\Sviluppo\jims code locale\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0412F6D2-EA35-4349-A9FA-7D6BFE7CB449}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB8B5AD5-5095-404D-9A9A-BBF1A63AC4EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EB9272F1-67AB-4F1E-9686-A9D81288A326}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="17">
   <si>
     <t>Tipo 1</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>HH05HD</t>
+  </si>
+  <si>
+    <t>n other inverter</t>
   </si>
 </sst>
 </file>
@@ -225,20 +228,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -247,16 +244,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -573,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{313048AA-5A6B-4D72-AD89-8B09909A8CB9}">
-  <dimension ref="A1:L36"/>
+  <dimension ref="A1:L40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:I21"/>
+      <selection activeCell="A8" sqref="A8:I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -585,17 +585,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="5"/>
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="11"/>
       <c r="L1" t="s">
         <v>7</v>
       </c>
@@ -604,495 +604,626 @@
       <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="8"/>
+      <c r="B2" s="5">
+        <v>3</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="6"/>
+      <c r="L2">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="9"/>
+      <c r="B3" s="3">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="4"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="9"/>
+      <c r="B4" s="3">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="4"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="9"/>
+      <c r="B5" s="3">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="4"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="9"/>
+      <c r="B6" s="3">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="4"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="9"/>
+        <v>16</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="4"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="4"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="9"/>
-    </row>
-    <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="B9" s="3">
+        <v>0</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="4"/>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="9"/>
-    </row>
-    <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+      <c r="B10" s="3">
+        <v>0</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="4"/>
+    </row>
+    <row r="11" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="5"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="8"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="11"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="5">
+        <v>2</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="6"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="9"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="B13" s="3">
         <v>4</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="9"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="4"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="3">
+        <v>2</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="4"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="9"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="9"/>
+      <c r="B15" s="3">
+        <v>4</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="4"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="9"/>
+        <v>5</v>
+      </c>
+      <c r="B16" s="3">
+        <v>2</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="4"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3">
+        <v>0</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="4"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="3">
+        <v>0</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="4"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="9"/>
-    </row>
-    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+      <c r="B19" s="3">
+        <v>2</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="4"/>
+    </row>
+    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="9"/>
-    </row>
-    <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
+      <c r="B20" s="3">
+        <v>1</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="4"/>
+    </row>
+    <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="5"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="11"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="8"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="9"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="9"/>
+      <c r="B22" s="5">
+        <v>0</v>
+      </c>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="6"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>6</v>
-      </c>
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="9"/>
+        <v>9</v>
+      </c>
+      <c r="B23" s="3">
+        <v>0</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="4"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="9"/>
+        <v>4</v>
+      </c>
+      <c r="B24" s="3">
+        <v>0</v>
+      </c>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="4"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="9"/>
+      <c r="A25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="3">
+        <v>0</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="4"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="3">
+        <v>0</v>
+      </c>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="4"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" s="3">
+        <v>0</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="4"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" s="3">
+        <v>0</v>
+      </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="4"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="9"/>
-    </row>
-    <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
+      <c r="B29" s="3">
+        <v>0</v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="4"/>
+    </row>
+    <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="9"/>
-    </row>
-    <row r="28" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
+      <c r="B30" s="7">
+        <v>0</v>
+      </c>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="8"/>
+    </row>
+    <row r="31" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="5"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>12</v>
-      </c>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="8"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>9</v>
-      </c>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="9"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="9"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="11"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>6</v>
-      </c>
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="10"/>
-      <c r="I32" s="9"/>
+        <v>12</v>
+      </c>
+      <c r="B32" s="5">
+        <v>0</v>
+      </c>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="6"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B33" s="10"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="10"/>
-      <c r="I33" s="9"/>
+      <c r="A33" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" s="3">
+        <v>0</v>
+      </c>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="4"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="3">
+        <v>0</v>
+      </c>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="4"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="3">
+        <v>0</v>
+      </c>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="4"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" s="3">
+        <v>0</v>
+      </c>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="4"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B37" s="3">
+        <v>0</v>
+      </c>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="4"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="9"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+      <c r="B38" s="3">
+        <v>0</v>
+      </c>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="4"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="6"/>
-      <c r="I35" s="9"/>
-    </row>
-    <row r="36" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="2" t="s">
+      <c r="B39" s="3">
+        <v>0</v>
+      </c>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="4"/>
+    </row>
+    <row r="40" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B36" s="11"/>
-      <c r="C36" s="11"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="11"/>
-      <c r="F36" s="11"/>
-      <c r="G36" s="11"/>
-      <c r="H36" s="11"/>
-      <c r="I36" s="12"/>
+      <c r="B40" s="7">
+        <v>0</v>
+      </c>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="36">
-    <mergeCell ref="B33:I33"/>
-    <mergeCell ref="B34:I34"/>
-    <mergeCell ref="B35:I35"/>
-    <mergeCell ref="B36:I36"/>
-    <mergeCell ref="B27:I27"/>
-    <mergeCell ref="B29:I29"/>
-    <mergeCell ref="B30:I30"/>
-    <mergeCell ref="B31:I31"/>
-    <mergeCell ref="B32:I32"/>
-    <mergeCell ref="B22:I22"/>
-    <mergeCell ref="B23:I23"/>
-    <mergeCell ref="B24:I24"/>
-    <mergeCell ref="B25:I25"/>
-    <mergeCell ref="B26:I26"/>
-    <mergeCell ref="B16:I16"/>
-    <mergeCell ref="B17:I17"/>
-    <mergeCell ref="B18:I18"/>
-    <mergeCell ref="B20:I20"/>
-    <mergeCell ref="B21:I21"/>
-    <mergeCell ref="B11:I11"/>
-    <mergeCell ref="B12:I12"/>
-    <mergeCell ref="B13:I13"/>
-    <mergeCell ref="B14:I14"/>
-    <mergeCell ref="B15:I15"/>
+  <mergeCells count="40">
     <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="A19:I19"/>
-    <mergeCell ref="A28:I28"/>
+    <mergeCell ref="A11:I11"/>
+    <mergeCell ref="A21:I21"/>
+    <mergeCell ref="A31:I31"/>
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="B3:I3"/>
     <mergeCell ref="B4:I4"/>
     <mergeCell ref="B5:I5"/>
     <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B7:I7"/>
     <mergeCell ref="B8:I8"/>
     <mergeCell ref="B9:I9"/>
+    <mergeCell ref="B10:I10"/>
+    <mergeCell ref="B12:I12"/>
+    <mergeCell ref="B13:I13"/>
+    <mergeCell ref="B14:I14"/>
+    <mergeCell ref="B15:I15"/>
+    <mergeCell ref="B38:I38"/>
+    <mergeCell ref="B39:I39"/>
+    <mergeCell ref="B40:I40"/>
+    <mergeCell ref="B30:I30"/>
+    <mergeCell ref="B32:I32"/>
+    <mergeCell ref="B33:I33"/>
+    <mergeCell ref="B34:I34"/>
+    <mergeCell ref="B35:I35"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B17:I17"/>
+    <mergeCell ref="B27:I27"/>
+    <mergeCell ref="B37:I37"/>
+    <mergeCell ref="B29:I29"/>
+    <mergeCell ref="B36:I36"/>
+    <mergeCell ref="B23:I23"/>
+    <mergeCell ref="B24:I24"/>
+    <mergeCell ref="B25:I25"/>
+    <mergeCell ref="B26:I26"/>
+    <mergeCell ref="B28:I28"/>
+    <mergeCell ref="B16:I16"/>
+    <mergeCell ref="B18:I18"/>
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="B20:I20"/>
+    <mergeCell ref="B22:I22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
versione finale funzionante: rimossa la ibrida e acquisizione dati nel main da file excel_sviluppo
</commit_message>
<xml_diff>
--- a/excel_sviluppo.xlsx
+++ b/excel_sviluppo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Commesse\Sviluppo\jims code locale\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB8B5AD5-5095-404D-9A9A-BBF1A63AC4EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE620FFE-E4E6-4C62-BD91-FEFC87950402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EB9272F1-67AB-4F1E-9686-A9D81288A326}"/>
+    <workbookView xWindow="0" yWindow="2160" windowWidth="21600" windowHeight="11385" xr2:uid="{EB9272F1-67AB-4F1E-9686-A9D81288A326}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="15">
   <si>
     <t>Tipo 1</t>
   </si>
@@ -62,19 +62,7 @@
     <t>n tot PI</t>
   </si>
   <si>
-    <t>n tipo 1</t>
-  </si>
-  <si>
     <t>n HVAC</t>
-  </si>
-  <si>
-    <t>n tipo 2</t>
-  </si>
-  <si>
-    <t>n tipo 3</t>
-  </si>
-  <si>
-    <t>n tipo 4</t>
   </si>
   <si>
     <t>EH05HD</t>
@@ -83,10 +71,16 @@
     <t>PH2HD</t>
   </si>
   <si>
-    <t>HH05HD</t>
+    <t>n other inverter</t>
   </si>
   <si>
-    <t>n other inverter</t>
+    <t>spare</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n tipo </t>
   </si>
 </sst>
 </file>
@@ -110,7 +104,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -134,17 +128,6 @@
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -238,13 +221,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -254,9 +240,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -573,15 +556,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{313048AA-5A6B-4D72-AD89-8B09909A8CB9}">
-  <dimension ref="A1:L40"/>
+  <dimension ref="A1:L52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:I8"/>
+      <selection activeCell="B22" sqref="B22:I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.85546875" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -602,28 +587,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="5">
+        <v>14</v>
+      </c>
+      <c r="B2" s="7">
         <v>3</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="6"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="8"/>
       <c r="L2">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -638,7 +623,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -653,7 +638,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -668,7 +653,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -680,10 +665,10 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B7" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -695,10 +680,10 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B8" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -709,11 +694,11 @@
       <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>13</v>
+      <c r="A9" t="s">
+        <v>10</v>
       </c>
       <c r="B9" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -723,12 +708,12 @@
       <c r="H9" s="3"/>
       <c r="I9" s="4"/>
     </row>
-    <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="3">
-        <v>0</v>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -738,85 +723,85 @@
       <c r="H10" s="3"/>
       <c r="I10" s="4"/>
     </row>
-    <row r="11" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="11"/>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="4"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="5">
-        <v>2</v>
-      </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="6"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="4"/>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="3">
-        <v>4</v>
-      </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="4"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="3">
-        <v>2</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="4"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="6"/>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="11"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="3">
+        <v>14</v>
+      </c>
+      <c r="B15" s="7">
+        <v>2</v>
+      </c>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="8"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="3">
         <v>4</v>
-      </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="4"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="3">
-        <v>2</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -828,10 +813,10 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B17" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
@@ -842,11 +827,11 @@
       <c r="I17" s="4"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>15</v>
+      <c r="A18" t="s">
+        <v>6</v>
       </c>
       <c r="B18" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -858,7 +843,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B19" s="3">
         <v>2</v>
@@ -871,9 +856,9 @@
       <c r="H19" s="3"/>
       <c r="I19" s="4"/>
     </row>
-    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>14</v>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="B20" s="3">
         <v>1</v>
@@ -886,40 +871,42 @@
       <c r="H20" s="3"/>
       <c r="I20" s="4"/>
     </row>
-    <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="9" t="s">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="3">
         <v>2</v>
       </c>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="11"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="4"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>11</v>
-      </c>
-      <c r="B22" s="5">
-        <v>0</v>
-      </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="6"/>
+        <v>10</v>
+      </c>
+      <c r="B22" s="3">
+        <v>1</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="4"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>9</v>
-      </c>
-      <c r="B23" s="3">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
@@ -930,11 +917,11 @@
       <c r="I23" s="4"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B24" s="3">
-        <v>0</v>
+      <c r="A24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -946,10 +933,10 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>6</v>
-      </c>
-      <c r="B25" s="3">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -959,54 +946,52 @@
       <c r="H25" s="3"/>
       <c r="I25" s="4"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B26" s="3">
-        <v>0</v>
-      </c>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="4"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B27" s="3">
-        <v>0</v>
-      </c>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="4"/>
+    <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="6"/>
+    </row>
+    <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="11"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B28" s="3">
-        <v>0</v>
-      </c>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="4"/>
+      <c r="A28" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" s="7">
+        <v>3</v>
+      </c>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="8"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>13</v>
+      <c r="A29" t="s">
+        <v>8</v>
       </c>
       <c r="B29" s="3">
         <v>0</v>
@@ -1019,55 +1004,57 @@
       <c r="H29" s="3"/>
       <c r="I29" s="4"/>
     </row>
-    <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B30" s="7">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" s="3">
         <v>0</v>
       </c>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="8"/>
-    </row>
-    <row r="31" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="10"/>
-      <c r="I31" s="11"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="4"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" s="3">
+        <v>0</v>
+      </c>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="4"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>12</v>
-      </c>
-      <c r="B32" s="5">
+      <c r="A32" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="3">
         <v>0</v>
       </c>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
-      <c r="I32" s="6"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="4"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>9</v>
+      <c r="A33" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="B33" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
@@ -1079,10 +1066,10 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B34" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
@@ -1094,7 +1081,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B35" s="3">
         <v>0</v>
@@ -1108,11 +1095,11 @@
       <c r="I35" s="4"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B36" s="3">
-        <v>0</v>
+      <c r="A36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
@@ -1123,11 +1110,11 @@
       <c r="I36" s="4"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B37" s="3">
-        <v>0</v>
+      <c r="A37" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
@@ -1138,11 +1125,11 @@
       <c r="I37" s="4"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B38" s="3">
-        <v>0</v>
+      <c r="A38" t="s">
+        <v>12</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
@@ -1152,78 +1139,268 @@
       <c r="H38" s="3"/>
       <c r="I38" s="4"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B39" s="3">
+    <row r="39" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>12</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="6"/>
+    </row>
+    <row r="40" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B40" s="10"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="11"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>14</v>
+      </c>
+      <c r="B41" s="7">
+        <v>3</v>
+      </c>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7"/>
+      <c r="I41" s="8"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>8</v>
+      </c>
+      <c r="B42" s="3">
         <v>0</v>
       </c>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="4"/>
-    </row>
-    <row r="40" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B40" s="7">
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="4"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43" s="3">
         <v>0</v>
       </c>
-      <c r="C40" s="7"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
-      <c r="G40" s="7"/>
-      <c r="H40" s="7"/>
-      <c r="I40" s="8"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="4"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44" s="3">
+        <v>0</v>
+      </c>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="4"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B45" s="3">
+        <v>0</v>
+      </c>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3"/>
+      <c r="I45" s="4"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B46" s="3">
+        <v>1</v>
+      </c>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
+      <c r="I46" s="4"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B47" s="3">
+        <v>2</v>
+      </c>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="4"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>10</v>
+      </c>
+      <c r="B48" s="3">
+        <v>0</v>
+      </c>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="3"/>
+      <c r="I48" s="4"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>12</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="3"/>
+      <c r="I49" s="4"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>12</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3"/>
+      <c r="H50" s="3"/>
+      <c r="I50" s="4"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>12</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="3"/>
+      <c r="I51" s="4"/>
+    </row>
+    <row r="52" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
+      <c r="G52" s="5"/>
+      <c r="H52" s="5"/>
+      <c r="I52" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="40">
+  <mergeCells count="52">
+    <mergeCell ref="A40:I40"/>
     <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A11:I11"/>
-    <mergeCell ref="A21:I21"/>
-    <mergeCell ref="A31:I31"/>
+    <mergeCell ref="A14:I14"/>
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="B3:I3"/>
     <mergeCell ref="B4:I4"/>
     <mergeCell ref="B5:I5"/>
     <mergeCell ref="B6:I6"/>
     <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B9:I9"/>
-    <mergeCell ref="B10:I10"/>
     <mergeCell ref="B12:I12"/>
     <mergeCell ref="B13:I13"/>
-    <mergeCell ref="B14:I14"/>
     <mergeCell ref="B15:I15"/>
-    <mergeCell ref="B38:I38"/>
+    <mergeCell ref="B16:I16"/>
+    <mergeCell ref="B18:I18"/>
+    <mergeCell ref="B24:I24"/>
+    <mergeCell ref="B35:I35"/>
     <mergeCell ref="B39:I39"/>
-    <mergeCell ref="B40:I40"/>
-    <mergeCell ref="B30:I30"/>
-    <mergeCell ref="B32:I32"/>
+    <mergeCell ref="B31:I31"/>
     <mergeCell ref="B33:I33"/>
     <mergeCell ref="B34:I34"/>
-    <mergeCell ref="B35:I35"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B17:I17"/>
-    <mergeCell ref="B27:I27"/>
+    <mergeCell ref="B36:I36"/>
+    <mergeCell ref="B32:I32"/>
+    <mergeCell ref="A27:I27"/>
+    <mergeCell ref="B29:I29"/>
+    <mergeCell ref="B38:I38"/>
+    <mergeCell ref="B30:I30"/>
     <mergeCell ref="B37:I37"/>
-    <mergeCell ref="B29:I29"/>
-    <mergeCell ref="B36:I36"/>
-    <mergeCell ref="B23:I23"/>
-    <mergeCell ref="B24:I24"/>
     <mergeCell ref="B25:I25"/>
     <mergeCell ref="B26:I26"/>
     <mergeCell ref="B28:I28"/>
-    <mergeCell ref="B16:I16"/>
-    <mergeCell ref="B18:I18"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B10:I10"/>
+    <mergeCell ref="B11:I11"/>
+    <mergeCell ref="B23:I23"/>
+    <mergeCell ref="B9:I9"/>
+    <mergeCell ref="B20:I20"/>
     <mergeCell ref="B19:I19"/>
-    <mergeCell ref="B20:I20"/>
+    <mergeCell ref="B17:I17"/>
+    <mergeCell ref="B21:I21"/>
     <mergeCell ref="B22:I22"/>
+    <mergeCell ref="B41:I41"/>
+    <mergeCell ref="B42:I42"/>
+    <mergeCell ref="B43:I43"/>
+    <mergeCell ref="B44:I44"/>
+    <mergeCell ref="B45:I45"/>
+    <mergeCell ref="B51:I51"/>
+    <mergeCell ref="B52:I52"/>
+    <mergeCell ref="B46:I46"/>
+    <mergeCell ref="B47:I47"/>
+    <mergeCell ref="B48:I48"/>
+    <mergeCell ref="B49:I49"/>
+    <mergeCell ref="B50:I50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>